<commit_message>
map and updated score schema
drop geom in score schema, added score map
</commit_message>
<xml_diff>
--- a/csv/Book1.xlsx
+++ b/csv/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sherryfan/Documents/GitHub/covid-19_vulnerability_analysis_nsw/csv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D07D4B97-9526-904B-B77F-C69EF8D36F74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F49C3A-8D1F-1D43-9C7B-579200FEF8A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{F37FE858-2CA8-6147-A3AF-F5771A9DF5A5}"/>
   </bookViews>
@@ -114,7 +114,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -123,26 +123,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
+      <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="12"/>
+      <sz val="10"/>
       <color rgb="FF8C7252"/>
-      <name val="Calibri (Body)"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
-      <sz val="12"/>
-      <color rgb="FF8C7252"/>
-      <name val="Calibri"/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -153,7 +151,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -198,25 +196,108 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -536,198 +617,287 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54B4AFDA-3D3B-8347-8C02-A2F8395D96EE}">
-  <dimension ref="C9:H38"/>
+  <dimension ref="B7:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="141" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="1.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="1.1640625" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="9" spans="4:8">
-      <c r="D9" s="6" t="s">
+    <row r="7" spans="2:10" ht="14" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="2:10" ht="5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B8" s="2"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="4"/>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B9" s="5"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="E9" s="6"/>
+      <c r="F9" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="G9" s="6"/>
+      <c r="H9" s="7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="4:8">
-      <c r="D10" s="3"/>
-      <c r="F10" s="5"/>
-      <c r="H10" s="3"/>
-    </row>
-    <row r="11" spans="4:8">
-      <c r="D11" s="3" t="s">
+      <c r="I9" s="6"/>
+      <c r="J9" s="8"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B10" s="5"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="E10" s="6"/>
+      <c r="F10" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="G10" s="6"/>
+      <c r="H10" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="4:8">
-      <c r="D12" s="3" t="s">
+      <c r="I10" s="6"/>
+      <c r="J10" s="8"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B11" s="5"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="E11" s="6"/>
+      <c r="F11" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="G11" s="6"/>
+      <c r="H11" s="11" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="4:8">
-      <c r="D13" s="3" t="s">
+      <c r="I11" s="6"/>
+      <c r="J11" s="8"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B12" s="5"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="E12" s="6"/>
+      <c r="F12" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="H13" s="4"/>
-    </row>
-    <row r="14" spans="4:8">
-      <c r="D14" s="3" t="s">
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="8"/>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B13" s="5"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F14" s="4"/>
-    </row>
-    <row r="15" spans="4:8">
-      <c r="D15" s="4"/>
-    </row>
-    <row r="16" spans="4:8">
-      <c r="D16" s="7"/>
-    </row>
-    <row r="18" spans="3:7">
-      <c r="C18" s="6" t="s">
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="8"/>
+    </row>
+    <row r="14" spans="2:10" ht="4" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B14" s="5"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="8"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B15" s="5"/>
+      <c r="C15" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="D15" s="6"/>
+      <c r="E15" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G18" s="6" t="s">
+      <c r="F15" s="6"/>
+      <c r="G15" s="7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="19" spans="3:7">
-      <c r="C19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="G19" s="3"/>
-    </row>
-    <row r="20" spans="3:7">
-      <c r="C20" s="2" t="s">
+      <c r="H15" s="6"/>
+      <c r="I15" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J15" s="8"/>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B16" s="5"/>
+      <c r="C16" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="D16" s="6"/>
+      <c r="E16" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="F16" s="6"/>
+      <c r="G16" s="10" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="21" spans="3:7">
-      <c r="C21" s="3" t="s">
+      <c r="H16" s="6"/>
+      <c r="I16" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="J16" s="8"/>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B17" s="5"/>
+      <c r="C17" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="D17" s="6"/>
+      <c r="E17" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="F17" s="6"/>
+      <c r="G17" s="11" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="3:7">
-      <c r="C22" s="3" t="s">
+      <c r="H17" s="6"/>
+      <c r="I17" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="J17" s="8"/>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B18" s="5"/>
+      <c r="C18" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="D18" s="6"/>
+      <c r="E18" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G22" s="4"/>
-    </row>
-    <row r="23" spans="3:7">
-      <c r="C23" s="3" t="s">
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="J18" s="8"/>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B19" s="5"/>
+      <c r="C19" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E23" s="4"/>
-    </row>
-    <row r="24" spans="3:7">
-      <c r="C24" s="3" t="s">
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="J19" s="8"/>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B20" s="5"/>
+      <c r="C20" s="9" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="25" spans="3:7">
-      <c r="C25" s="3" t="s">
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J20" s="8"/>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B21" s="5"/>
+      <c r="C21" s="9" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="26" spans="3:7">
-      <c r="C26" s="3" t="s">
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="J21" s="8"/>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B22" s="5"/>
+      <c r="C22" s="9" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="27" spans="3:7">
-      <c r="C27" s="3" t="s">
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="8"/>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B23" s="5"/>
+      <c r="C23" s="11" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="28" spans="3:7">
-      <c r="C28" s="4"/>
-    </row>
-    <row r="30" spans="3:7">
-      <c r="E30" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="31" spans="3:7">
-      <c r="E31" s="3"/>
-    </row>
-    <row r="32" spans="3:7">
-      <c r="E32" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="5:5">
-      <c r="E33" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="5:5">
-      <c r="E34" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="5:5">
-      <c r="E35" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="36" spans="5:5">
-      <c r="E36" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="37" spans="5:5">
-      <c r="E37" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="38" spans="5:5">
-      <c r="E38" s="4"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="8"/>
+    </row>
+    <row r="24" spans="2:10" ht="5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="12"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>